<commit_message>
Updated Spreadsheet... Needs work in MS Excel
</commit_message>
<xml_diff>
--- a/PA2/Data.xlsx
+++ b/PA2/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,11 @@
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequential-Dynamic'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequential-Static'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Raw!$A$1:$D$454</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Raw!$A$1:$D$395</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Raw!$A$1:$D$454</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Raw!$A$1:$D$395</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Averaged Data'!$A$1:$D$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequential-Static'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequential-Dynamic'!$A$1:$D$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -436,7 +440,7 @@
   <dimension ref="A1:D454"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="B1:D41 E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -444,7 +448,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.42"/>
@@ -6832,12 +6836,12 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G63" activeCellId="0" sqref="G63"/>
+      <selection pane="topLeft" activeCell="G63" activeCellId="1" sqref="B1:D41 G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
@@ -7927,8 +7931,8 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8533,13 +8537,13 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="B1:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.39"/>

</xml_diff>

<commit_message>
Data ready for graphing
</commit_message>
<xml_diff>
--- a/PA2/Data.xlsx
+++ b/PA2/Data.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Averaged Data" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sequential-Static" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sequential-Dynamic" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Graphs" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Averaged Data'!$A$1:$D$76</definedName>
@@ -20,10 +21,14 @@
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequential-Static'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Raw!$A$1:$D$454</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Raw!$A$1:$D$454</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Raw!$A$1:$D$395</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Raw!$A$1:$D$454</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Raw!$A$1:$D$395</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Averaged Data'!$A$1:$D$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Averaged Data'!$A$1:$D$76</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequential-Static'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sequential-Static'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequential-Dynamic'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sequential-Dynamic'!$A$1:$D$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -35,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="14">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -59,6 +64,24 @@
   </si>
   <si>
     <t xml:space="preserve">Image Dimensions (square images)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequential Static</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cores | Image Dimensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequential Dynamic</t>
   </si>
 </sst>
 </file>
@@ -440,7 +463,7 @@
   <dimension ref="A1:D454"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="B1:D41 E13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6836,12 +6859,12 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G63" activeCellId="1" sqref="B1:D41 G63"/>
+      <selection pane="topLeft" activeCell="G63" activeCellId="0" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
@@ -7931,8 +7954,8 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:D41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8538,7 +8561,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="B1:D41"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9135,4 +9158,1149 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Z24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R26" activeCellId="0" sqref="R26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.0539536666666667</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.817115333333333</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>13.1197333333333</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>52.1525833333333</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>209.9145</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <f aca="false"> D$5 / D6</f>
+        <v>1.67905601659751</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <f aca="false"> E$5 / E6</f>
+        <v>1.9770489833265</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <f aca="false"> F$5 / F6</f>
+        <v>2.03335682211279</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <f aca="false"> G$5 / G6</f>
+        <v>2.02043645464219</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <f aca="false"> H$5 / H6</f>
+        <v>2.03363812654704</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <f aca="false">D$5/(D6 * $C6)</f>
+        <v>0.559685338865838</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <f aca="false">E$5/(E6 * $C6)</f>
+        <v>0.659016327775499</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <f aca="false">F$5/(F6 * $C6)</f>
+        <v>0.677785607370929</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <f aca="false">G$5/(G6 * $C6)</f>
+        <v>0.673478818214064</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <f aca="false">H$5/(H6 * $C6)</f>
+        <v>0.677879375515678</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.0321333333333333</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.4133005</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>6.45225333333333</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>25.8125333333333</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>103.221166666667</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false"> D$5 / D7</f>
+        <v>1.73965520947529</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <f aca="false"> E$5 / E7</f>
+        <v>2.01343579516614</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <f aca="false"> F$5 / F7</f>
+        <v>2.02221657629617</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <f aca="false"> G$5 / G7</f>
+        <v>2.01189007355991</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <f aca="false"> H$5 / H7</f>
+        <v>2.03654170789918</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <f aca="false">D$5/(D7 * $C7)</f>
+        <v>0.217456901184411</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <f aca="false">E$5/(E7 * $C7)</f>
+        <v>0.251679474395767</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <f aca="false">F$5/(F7 * $C7)</f>
+        <v>0.252777072037021</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <f aca="false">G$5/(G7 * $C7)</f>
+        <v>0.251486259194988</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <f aca="false">H$5/(H7 * $C7)</f>
+        <v>0.254567713487397</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.031014</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.405831333333333</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>6.48779833333333</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>25.9221833333333</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>103.074</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false"> D$5 / D8</f>
+        <v>2.04965176649361</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <f aca="false"> E$5 / E8</f>
+        <v>2.59938348908699</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <f aca="false"> F$5 / F8</f>
+        <v>2.69576729904789</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <f aca="false"> G$5 / G8</f>
+        <v>2.68147704447141</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <f aca="false"> H$5 / H8</f>
+        <v>2.69853621914354</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <f aca="false">D$5/(D8 * $C8)</f>
+        <v>0.227739085165957</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <f aca="false">E$5/(E8 * $C8)</f>
+        <v>0.288820387676332</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <f aca="false">F$5/(F8 * $C8)</f>
+        <v>0.29952969989421</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <f aca="false">G$5/(G8 * $C8)</f>
+        <v>0.297941893830156</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <f aca="false">H$5/(H8 * $C8)</f>
+        <v>0.299837357682616</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.0263233333333333</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.314349666666667</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>4.86679</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>19.4492</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>77.7882833333333</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false"> D$5 / D9</f>
+        <v>1.75666641343159</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <f aca="false"> E$5 / E9</f>
+        <v>3.294602909217</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <f aca="false"> F$5 / F9</f>
+        <v>3.5918020197909</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <f aca="false"> G$5 / G9</f>
+        <v>3.55648842294769</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <f aca="false"> H$5 / H9</f>
+        <v>3.57470732934676</v>
+      </c>
+      <c r="U8" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <f aca="false">D$5/(D9 * $C9)</f>
+        <v>0.135128185648584</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <f aca="false">E$5/(E9 * $C9)</f>
+        <v>0.253430993016693</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <f aca="false">F$5/(F9 * $C9)</f>
+        <v>0.276292463060838</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <f aca="false">G$5/(G9 * $C9)</f>
+        <v>0.273576032534438</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <f aca="false">H$5/(H9 * $C9)</f>
+        <v>0.274977486872828</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.0307136666666667</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.248016333333333</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>3.65268833333333</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>14.6640666666667</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>58.72215</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <f aca="false"> D$5 / D10</f>
+        <v>1.21012593874644</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <f aca="false"> E$5 / E10</f>
+        <v>3.56022665465084</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <f aca="false"> F$5 / F10</f>
+        <v>3.96196995243726</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <f aca="false"> G$5 / G10</f>
+        <v>3.97779334296059</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <f aca="false"> H$5 / H10</f>
+        <v>3.98477512285067</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <f aca="false">D$5/(D10 * $C10)</f>
+        <v>0.0756328711716528</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <f aca="false">E$5/(E10 * $C10)</f>
+        <v>0.222514165915677</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <f aca="false">F$5/(F10 * $C10)</f>
+        <v>0.247623122027329</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <f aca="false">G$5/(G10 * $C10)</f>
+        <v>0.248612083935037</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <f aca="false">H$5/(H10 * $C10)</f>
+        <v>0.249048445178167</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.0445851666666667</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.229512166666667</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>3.31141666666667</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>13.1109333333333</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>52.6791333333333</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false"> D$5 / D11</f>
+        <v>1.86463991336954</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <f aca="false"> E$5 / E11</f>
+        <v>3.88673412506691</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <f aca="false"> F$5 / F11</f>
+        <v>4.51324013883999</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <f aca="false"> G$5 / G11</f>
+        <v>4.488637667688</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <f aca="false"> H$5 / H11</f>
+        <v>4.52812300802775</v>
+      </c>
+      <c r="U10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <f aca="false">D$5/(D11 * $C11)</f>
+        <v>0.109684700786444</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <f aca="false">E$5/(E11 * $C11)</f>
+        <v>0.228631419121583</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <f aca="false">F$5/(F11 * $C11)</f>
+        <v>0.265484714049411</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <f aca="false">G$5/(G11 * $C11)</f>
+        <v>0.264037509864</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <f aca="false">H$5/(H11 * $C11)</f>
+        <v>0.266360176942809</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.0289351666666667</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.210231857142857</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>2.90694333333333</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>11.6188</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>46.35795</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <f aca="false"> D$5 / D12</f>
+        <v>0.955044843049329</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <f aca="false"> E$5 / E12</f>
+        <v>1.43837947849527</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <f aca="false"> F$5 / F12</f>
+        <v>7.20058688903074</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <f aca="false"> G$5 / G12</f>
+        <v>8.00143144117845</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <f aca="false"> H$5 / H12</f>
+        <v>8.08270174875663</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <f aca="false">D$5/(D12 * $C12)</f>
+        <v>0.0298451513452915</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <f aca="false">E$5/(E12 * $C12)</f>
+        <v>0.0449493587029772</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <f aca="false">F$5/(F12 * $C12)</f>
+        <v>0.225018340282211</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <f aca="false">G$5/(G12 * $C12)</f>
+        <v>0.250044732536826</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <f aca="false">H$5/(H12 * $C12)</f>
+        <v>0.252584429648645</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.0564933333333333</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.5680805</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1.82203666666667</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>6.51790666666667</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>25.9708333333333</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="U16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.0539536666666667</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0.817115333333333</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>13.1197333333333</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>52.1525833333333</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>209.9145</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <f aca="false">D$17 / D18</f>
+        <v>1.77440254330191</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <f aca="false">E$17 / E18</f>
+        <v>1.97243486894936</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <f aca="false">F$17 / F18</f>
+        <v>2.02269929980086</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <f aca="false">G$17 / G18</f>
+        <v>2.01362491803363</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <f aca="false">H$17 / H18</f>
+        <v>2.00220491216914</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <f aca="false">D$17/(D18*$C18)</f>
+        <v>0.591467514433969</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <f aca="false">E$17/(E18*$C18)</f>
+        <v>0.657478289649786</v>
+      </c>
+      <c r="X17" s="0" t="n">
+        <f aca="false">F$17/(F18*$C18)</f>
+        <v>0.674233099933618</v>
+      </c>
+      <c r="Y17" s="0" t="n">
+        <f aca="false">G$17/(G18*$C18)</f>
+        <v>0.67120830601121</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <f aca="false">H$17/(H18*$C18)</f>
+        <v>0.667401637389713</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0.0304066666666667</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0.414267333333333</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>6.48625</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>25.89985</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>104.841666666667</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <f aca="false">D$17 / D19</f>
+        <v>5.32402473521479</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <f aca="false">E$17 / E19</f>
+        <v>6.8753069401069</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <f aca="false">F$17 / F19</f>
+        <v>7.03891781592389</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <f aca="false">G$17 / G19</f>
+        <v>7.00454948584363</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <f aca="false">H$17 / H19</f>
+        <v>7.00635947028148</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <f aca="false">D$17/(D19*$C19)</f>
+        <v>0.665503091901849</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <f aca="false">E$17/(E19*$C19)</f>
+        <v>0.859413367513363</v>
+      </c>
+      <c r="X18" s="0" t="n">
+        <f aca="false">F$17/(F19*$C19)</f>
+        <v>0.879864726990486</v>
+      </c>
+      <c r="Y18" s="0" t="n">
+        <f aca="false">G$17/(G19*$C19)</f>
+        <v>0.875568685730453</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <f aca="false">H$17/(H19*$C19)</f>
+        <v>0.875794933785186</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0.010134</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.118847833333333</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1.863885</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>7.44553</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>29.9605666666667</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <f aca="false">D$17 / D20</f>
+        <v>3.6141788545272</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <f aca="false">E$17 / E20</f>
+        <v>6.47806726619749</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <f aca="false">F$17 / F20</f>
+        <v>7.57381784174517</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <f aca="false">G$17 / G20</f>
+        <v>7.71442461847046</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <f aca="false">H$17 / H20</f>
+        <v>7.81426125153557</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <f aca="false">D$17/(D20*$C20)</f>
+        <v>0.4015754282808</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <f aca="false">E$17/(E20*$C20)</f>
+        <v>0.719785251799721</v>
+      </c>
+      <c r="X19" s="0" t="n">
+        <f aca="false">F$17/(F20*$C20)</f>
+        <v>0.841535315749463</v>
+      </c>
+      <c r="Y19" s="0" t="n">
+        <f aca="false">G$17/(G20*$C20)</f>
+        <v>0.857158290941162</v>
+      </c>
+      <c r="Z19" s="0" t="n">
+        <f aca="false">H$17/(H20*$C20)</f>
+        <v>0.868251250170619</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0.0149283333333333</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.126135666666667</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1.73224833333333</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>6.76039833333333</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>26.863</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <f aca="false">D$17 / D21</f>
+        <v>3.07586036523954</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <f aca="false">E$17 / E21</f>
+        <v>8.96948208643662</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <f aca="false">F$17 / F21</f>
+        <v>11.0325264326318</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <f aca="false">G$17 / G21</f>
+        <v>11.2281333157271</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <f aca="false">H$17 / H21</f>
+        <v>11.5100269407778</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <f aca="false">D$17/(D21*$C21)</f>
+        <v>0.236604643479964</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <f aca="false">E$17/(E21*$C21)</f>
+        <v>0.689960160495125</v>
+      </c>
+      <c r="X20" s="0" t="n">
+        <f aca="false">F$17/(F21*$C21)</f>
+        <v>0.848655879433213</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <f aca="false">G$17/(G21*$C21)</f>
+        <v>0.863702562748237</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <f aca="false">H$17/(H21*$C21)</f>
+        <v>0.885386687752141</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0.017541</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.0910995</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1.18918666666667</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>4.64481333333333</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>18.2375333333333</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <f aca="false">D$17 / D22</f>
+        <v>1.16440061003683</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <f aca="false">E$17 / E22</f>
+        <v>9.65613871994454</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <f aca="false">F$17 / F22</f>
+        <v>13.51840924656</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <f aca="false">G$17 / G22</f>
+        <v>13.846124914268</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <f aca="false">H$17 / H22</f>
+        <v>13.6318001413523</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="V21" s="0" t="n">
+        <f aca="false">D$17/(D22*$C22)</f>
+        <v>0.0727750381273021</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <f aca="false">E$17/(E22*$C22)</f>
+        <v>0.603508669996534</v>
+      </c>
+      <c r="X21" s="0" t="n">
+        <f aca="false">F$17/(F22*$C22)</f>
+        <v>0.844900577910002</v>
+      </c>
+      <c r="Y21" s="0" t="n">
+        <f aca="false">G$17/(G22*$C22)</f>
+        <v>0.865382807141751</v>
+      </c>
+      <c r="Z21" s="0" t="n">
+        <f aca="false">H$17/(H22*$C22)</f>
+        <v>0.851987508834517</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0.046336</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0.0846213333333333</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0.970508666666666</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>3.76658333333333</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>15.3988833333333</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <f aca="false">D$17 / D23</f>
+        <v>1.63773878905618</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <f aca="false">E$17 / E23</f>
+        <v>9.16941192753034</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <f aca="false">F$17 / F23</f>
+        <v>1.7594678931933</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <f aca="false">G$17 / G23</f>
+        <v>0.845295376795589</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <f aca="false">H$17 / H23</f>
+        <v>1.33440729773111</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="V22" s="0" t="n">
+        <f aca="false">D$17/(D23*$C23)</f>
+        <v>0.0963375758268339</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <f aca="false">E$17/(E23*$C23)</f>
+        <v>0.539377172207667</v>
+      </c>
+      <c r="X22" s="0" t="n">
+        <f aca="false">F$17/(F23*$C23)</f>
+        <v>0.103498111364312</v>
+      </c>
+      <c r="Y22" s="0" t="n">
+        <f aca="false">G$17/(G23*$C23)</f>
+        <v>0.049723257458564</v>
+      </c>
+      <c r="Z22" s="0" t="n">
+        <f aca="false">H$17/(H23*$C23)</f>
+        <v>0.0784945469253594</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0.032944</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.0891131666666667</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>7.45664833333333</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>61.6974666666667</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>157.309166666667</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <f aca="false">D$17 / D24</f>
+        <v>0.838375676585606</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <f aca="false">E$17 / E24</f>
+        <v>8.90888309422785</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <f aca="false">F$17 / F24</f>
+        <v>0.343669082556911</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <f aca="false">G$17 / G24</f>
+        <v>0.613973333019396</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <f aca="false">H$17 / H24</f>
+        <v>1.07326665007823</v>
+      </c>
+      <c r="U23" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="V23" s="0" t="n">
+        <f aca="false">D$17/(D24*$C24)</f>
+        <v>0.0261992398933002</v>
+      </c>
+      <c r="W23" s="0" t="n">
+        <f aca="false">E$17/(E24*$C24)</f>
+        <v>0.27840259669462</v>
+      </c>
+      <c r="X23" s="0" t="n">
+        <f aca="false">F$17/(F24*$C24)</f>
+        <v>0.0107396588299035</v>
+      </c>
+      <c r="Y23" s="0" t="n">
+        <f aca="false">G$17/(G24*$C24)</f>
+        <v>0.0191866666568561</v>
+      </c>
+      <c r="Z23" s="0" t="n">
+        <f aca="false">H$17/(H24*$C24)</f>
+        <v>0.0335395828149445</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0.064355</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0.0917191666666667</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>38.1754833333333</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>84.94275</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>195.584666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>